<commit_message>
Added a rejected data check. Found and fixed error in difference vs total check. Updated Methods excel. Updated app so that rejected data is automatically included in data pull for verification and quality check purposes.
</commit_message>
<xml_diff>
--- a/2_21_19_QLs.xlsx
+++ b/2_21_19_QLs.xlsx
@@ -12,10 +12,10 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="19155" windowHeight="6870"/>
   </bookViews>
   <sheets>
-    <sheet name="QLs" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">QLs!$A$1:$H$191</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$191</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="539">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="509">
   <si>
     <t>Nitrates-Nitrite (as N)</t>
   </si>
@@ -1226,244 +1226,7 @@
     <t>Fluorotrichloromethane</t>
   </si>
   <si>
-    <t xml:space="preserve">SM4500-NO3 F, 353.2 </t>
-  </si>
-  <si>
-    <t>1632A</t>
-  </si>
-  <si>
-    <t>Calc</t>
-  </si>
-  <si>
-    <t>200.7, 200.8</t>
-  </si>
-  <si>
-    <t>335.4,  SM4500CN</t>
-  </si>
-  <si>
-    <t>SM4500CN-G, OIA</t>
-  </si>
-  <si>
-    <t>300.0, 300.1</t>
-  </si>
-  <si>
-    <t>SM4500-S</t>
-  </si>
-  <si>
-    <t>SM5540 C</t>
-  </si>
-  <si>
-    <t>625, 1625</t>
-  </si>
-  <si>
-    <t>625, 608</t>
-  </si>
-  <si>
-    <t>1657/508/622</t>
-  </si>
-  <si>
-    <t>614, 622</t>
-  </si>
-  <si>
-    <t>614, 622, 1657</t>
-  </si>
-  <si>
-    <t>614, 1657</t>
-  </si>
-  <si>
-    <t>505, 508, 608</t>
-  </si>
-  <si>
-    <t>505, 508, 608, 617</t>
-  </si>
-  <si>
-    <t>615, SM6640B</t>
-  </si>
-  <si>
-    <t>GCMS, SIM, GCFPD</t>
-  </si>
-  <si>
     <t>Min_WQ_Crit</t>
-  </si>
-  <si>
-    <t>DEQ_Pref_Method</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">625, 1625 , </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>604</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">625, 1625, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>609</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">625, 1625 (SIM), </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>610</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">625, 1625, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>611</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">625, 1625, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>612</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1631, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>245.7</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>625, 1625,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 607</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">625, 1625 (SIM), </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>604</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">625, 1625 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">(SIM), </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>610</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>625, 1625</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (SIM), </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>610</t>
-    </r>
   </si>
   <si>
     <t>Char_Name</t>
@@ -1802,17 +1565,10 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1855,7 +1611,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1865,23 +1621,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1889,15 +1645,15 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1909,14 +1665,14 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2249,28 +2005,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H191"/>
+  <dimension ref="A1:V191"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.5703125" style="2" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="40.140625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="37" style="4" customWidth="1"/>
     <col min="4" max="4" width="16.7109375" style="4" customWidth="1"/>
     <col min="5" max="5" width="12.140625" style="8" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="2"/>
-    <col min="7" max="7" width="13.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="36.7109375" style="8" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="2"/>
+    <col min="6" max="6" width="9.140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" style="8" customWidth="1"/>
+    <col min="23" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>430</v>
+        <v>400</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>369</v>
@@ -2288,15 +2044,12 @@
         <v>363</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>418</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>468</v>
+        <v>438</v>
       </c>
       <c r="B2" s="1">
         <v>959988</v>
@@ -2316,13 +2069,10 @@
       <c r="G2" s="8">
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="H2" s="8" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>469</v>
+        <v>439</v>
       </c>
       <c r="B3" s="1">
         <v>319846</v>
@@ -2342,13 +2092,10 @@
       <c r="G3" s="8">
         <v>4.4999999999999999E-4</v>
       </c>
-      <c r="H3" s="8" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>467</v>
+        <v>437</v>
       </c>
       <c r="B4" s="1">
         <v>33213659</v>
@@ -2368,13 +2115,10 @@
       <c r="G4" s="8">
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="H4" s="8" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>470</v>
+        <v>440</v>
       </c>
       <c r="B5" s="1">
         <v>319857</v>
@@ -2394,13 +2138,10 @@
       <c r="G5" s="8">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="H5" s="8" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>471</v>
+        <v>441</v>
       </c>
       <c r="B6" s="1">
         <v>71556</v>
@@ -2420,13 +2161,10 @@
       <c r="G6" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H6" s="8">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>472</v>
+        <v>442</v>
       </c>
       <c r="B7" s="1">
         <v>79345</v>
@@ -2446,13 +2184,10 @@
       <c r="G7" s="8">
         <v>0.12</v>
       </c>
-      <c r="H7" s="8">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>477</v>
+        <v>447</v>
       </c>
       <c r="B8" s="1">
         <v>79005</v>
@@ -2472,13 +2207,10 @@
       <c r="G8" s="8">
         <v>0.44</v>
       </c>
-      <c r="H8" s="8">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>478</v>
+        <v>448</v>
       </c>
       <c r="B9" s="1">
         <v>75343</v>
@@ -2498,13 +2230,10 @@
       <c r="G9" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H9" s="8">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>479</v>
+        <v>449</v>
       </c>
       <c r="B10" s="1">
         <v>75354</v>
@@ -2524,11 +2253,8 @@
       <c r="G10" s="8">
         <v>230</v>
       </c>
-      <c r="H10" s="8">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>370</v>
       </c>
@@ -2550,11 +2276,8 @@
       <c r="G11" s="8">
         <v>1.4E-3</v>
       </c>
-      <c r="H11" s="8" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>270</v>
       </c>
@@ -2576,13 +2299,10 @@
       <c r="G12" s="8">
         <v>0.11</v>
       </c>
-      <c r="H12" s="8" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>480</v>
+        <v>450</v>
       </c>
       <c r="B13" s="1">
         <v>120821</v>
@@ -2602,13 +2322,10 @@
       <c r="G13" s="8">
         <v>6.4</v>
       </c>
-      <c r="H13" s="8" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>481</v>
+        <v>451</v>
       </c>
       <c r="B14" s="1">
         <v>107062</v>
@@ -2628,13 +2345,10 @@
       <c r="G14" s="8">
         <v>0.35</v>
       </c>
-      <c r="H14" s="8">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>482</v>
+        <v>452</v>
       </c>
       <c r="B15" s="1">
         <v>78875</v>
@@ -2654,13 +2368,10 @@
       <c r="G15" s="8">
         <v>0.38</v>
       </c>
-      <c r="H15" s="8">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>483</v>
+        <v>453</v>
       </c>
       <c r="B16" s="1">
         <v>122667</v>
@@ -2680,11 +2391,8 @@
       <c r="G16" s="8">
         <v>1.4E-2</v>
       </c>
-      <c r="H16" s="8" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>371</v>
       </c>
@@ -2706,11 +2414,8 @@
       <c r="G17" s="8">
         <v>0.3</v>
       </c>
-      <c r="H17" s="8">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>383</v>
       </c>
@@ -2732,13 +2437,10 @@
       <c r="G18" s="8">
         <v>5.1E-10</v>
       </c>
-      <c r="H18" s="8">
-        <v>1613</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>484</v>
+        <v>454</v>
       </c>
       <c r="B19" s="1">
         <v>95954</v>
@@ -2758,13 +2460,10 @@
       <c r="G19" s="8">
         <v>330</v>
       </c>
-      <c r="H19" s="8" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>485</v>
+        <v>455</v>
       </c>
       <c r="B20" s="1">
         <v>88062</v>
@@ -2784,11 +2483,8 @@
       <c r="G20" s="8">
         <v>0.23</v>
       </c>
-      <c r="H20" s="14" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>379</v>
       </c>
@@ -2810,13 +2506,10 @@
       <c r="G21" s="8">
         <v>100</v>
       </c>
-      <c r="H21" s="14" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>508</v>
+        <v>478</v>
       </c>
       <c r="B22" s="1">
         <v>120832</v>
@@ -2836,13 +2529,10 @@
       <c r="G22" s="8">
         <v>23</v>
       </c>
-      <c r="H22" s="8" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>507</v>
+        <v>477</v>
       </c>
       <c r="B23" s="1">
         <v>105679</v>
@@ -2862,13 +2552,10 @@
       <c r="G23" s="8">
         <v>76</v>
       </c>
-      <c r="H23" s="8" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>509</v>
+        <v>479</v>
       </c>
       <c r="B24" s="1">
         <v>51285</v>
@@ -2888,13 +2575,10 @@
       <c r="G24" s="8">
         <v>62</v>
       </c>
-      <c r="H24" s="8" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>510</v>
+        <v>480</v>
       </c>
       <c r="B25" s="1">
         <v>121142</v>
@@ -2914,13 +2598,10 @@
       <c r="G25" s="8">
         <v>8.4000000000000005E-2</v>
       </c>
-      <c r="H25" s="14" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>511</v>
+        <v>481</v>
       </c>
       <c r="B26" s="1">
         <v>606202</v>
@@ -2940,13 +2621,10 @@
       <c r="G26" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H26" s="14" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>486</v>
+        <v>456</v>
       </c>
       <c r="B27" s="1">
         <v>110758</v>
@@ -2966,13 +2644,10 @@
       <c r="G27" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H27" s="8">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>512</v>
+        <v>482</v>
       </c>
       <c r="B28" s="1">
         <v>91587</v>
@@ -2992,13 +2667,10 @@
       <c r="G28" s="8">
         <v>150</v>
       </c>
-      <c r="H28" s="8" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>513</v>
+        <v>483</v>
       </c>
       <c r="B29" s="1">
         <v>91941</v>
@@ -3018,13 +2690,10 @@
       <c r="G29" s="8">
         <v>2.7000000000000001E-3</v>
       </c>
-      <c r="H29" s="8" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>514</v>
+        <v>484</v>
       </c>
       <c r="B30" s="1">
         <v>534521</v>
@@ -3044,11 +2713,8 @@
       <c r="G30" s="8">
         <v>9.1999999999999993</v>
       </c>
-      <c r="H30" s="8" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>180</v>
       </c>
@@ -3070,11 +2736,8 @@
       <c r="G31" s="8">
         <v>95</v>
       </c>
-      <c r="H31" s="14" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>182</v>
       </c>
@@ -3096,11 +2759,8 @@
       <c r="G32" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H32" s="14" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>88</v>
       </c>
@@ -3122,11 +2782,8 @@
       <c r="G33" s="8">
         <v>0.88</v>
       </c>
-      <c r="H33" s="8">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>90</v>
       </c>
@@ -3148,11 +2805,8 @@
       <c r="G34" s="8">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="H34" s="8">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>272</v>
       </c>
@@ -3174,11 +2828,8 @@
       <c r="G35" s="8">
         <v>5.0000000000000004E-6</v>
       </c>
-      <c r="H35" s="8" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>372</v>
       </c>
@@ -3200,13 +2851,10 @@
       <c r="G36" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H36" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>441</v>
+        <v>411</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>71</v>
@@ -3226,11 +2874,8 @@
       <c r="G37" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H37" s="8">
-        <v>200.8</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>184</v>
       </c>
@@ -3252,13 +2897,10 @@
       <c r="G38" s="8">
         <v>2900</v>
       </c>
-      <c r="H38" s="14" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>442</v>
+        <v>412</v>
       </c>
       <c r="B39" s="1">
         <v>7440360</v>
@@ -3278,13 +2920,10 @@
       <c r="G39" s="13">
         <v>5.0999999999999996</v>
       </c>
-      <c r="H39" s="8">
-        <v>200.8</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>487</v>
+        <v>457</v>
       </c>
       <c r="B40" s="1">
         <v>12674112</v>
@@ -3304,13 +2943,10 @@
       <c r="G40" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H40" s="8" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>488</v>
+        <v>458</v>
       </c>
       <c r="B41" s="1">
         <v>11104282</v>
@@ -3330,13 +2966,10 @@
       <c r="G41" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H41" s="8" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>489</v>
+        <v>459</v>
       </c>
       <c r="B42" s="1">
         <v>11141165</v>
@@ -3356,13 +2989,10 @@
       <c r="G42" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H42" s="8" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>490</v>
+        <v>460</v>
       </c>
       <c r="B43" s="1">
         <v>53469219</v>
@@ -3382,13 +3012,10 @@
       <c r="G43" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H43" s="8" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>491</v>
+        <v>461</v>
       </c>
       <c r="B44" s="1">
         <v>12672296</v>
@@ -3408,13 +3035,10 @@
       <c r="G44" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H44" s="8" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>492</v>
+        <v>462</v>
       </c>
       <c r="B45" s="1">
         <v>11097691</v>
@@ -3434,13 +3058,10 @@
       <c r="G45" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H45" s="8" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>493</v>
+        <v>463</v>
       </c>
       <c r="B46" s="1">
         <v>11096825</v>
@@ -3460,13 +3081,10 @@
       <c r="G46" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H46" s="8" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>465</v>
+        <v>435</v>
       </c>
       <c r="B47" s="2">
         <v>7440382</v>
@@ -3486,11 +3104,8 @@
       <c r="G47" s="13">
         <v>150</v>
       </c>
-      <c r="H47" s="14" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>373</v>
       </c>
@@ -3512,13 +3127,10 @@
       <c r="G48" s="13">
         <v>2.1</v>
       </c>
-      <c r="H48" s="14" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>443</v>
+        <v>413</v>
       </c>
       <c r="B49" s="2">
         <v>7440382</v>
@@ -3538,13 +3150,10 @@
       <c r="G49" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="H49" s="8">
-        <v>200.8</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>515</v>
+        <v>485</v>
       </c>
       <c r="B50" s="1">
         <v>86500</v>
@@ -3564,11 +3173,8 @@
       <c r="G50" s="8">
         <v>0.01</v>
       </c>
-      <c r="H50" s="14" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>186</v>
       </c>
@@ -3590,13 +3196,10 @@
       <c r="G51" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H51" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>444</v>
+        <v>414</v>
       </c>
       <c r="B52" s="15" t="s">
         <v>73</v>
@@ -3616,13 +3219,10 @@
       <c r="G52" s="8">
         <v>1000</v>
       </c>
-      <c r="H52" s="8">
-        <v>200.8</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>516</v>
+        <v>486</v>
       </c>
       <c r="B53" s="1">
         <v>56553</v>
@@ -3642,11 +3242,8 @@
       <c r="G53" s="8">
         <v>1.2999999999999999E-3</v>
       </c>
-      <c r="H53" s="14" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>92</v>
       </c>
@@ -3668,11 +3265,8 @@
       <c r="G54" s="8">
         <v>0.44</v>
       </c>
-      <c r="H54" s="8">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>374</v>
       </c>
@@ -3694,11 +3288,8 @@
       <c r="G55" s="8">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="H55" s="8" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>380</v>
       </c>
@@ -3720,11 +3311,8 @@
       <c r="G56" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H56" s="8" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>188</v>
       </c>
@@ -3746,11 +3334,8 @@
       <c r="G57" s="8">
         <v>1.8E-5</v>
       </c>
-      <c r="H57" s="8" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>194</v>
       </c>
@@ -3772,13 +3357,10 @@
       <c r="G58" s="8">
         <v>1.2999999999999999E-3</v>
       </c>
-      <c r="H58" s="14" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>517</v>
+        <v>487</v>
       </c>
       <c r="B59" s="1">
         <v>50328</v>
@@ -3798,13 +3380,10 @@
       <c r="G59" s="8">
         <v>1.2999999999999999E-3</v>
       </c>
-      <c r="H59" s="14" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>518</v>
+        <v>488</v>
       </c>
       <c r="B60" s="1">
         <v>191242</v>
@@ -3824,13 +3403,10 @@
       <c r="G60" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H60" s="14" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>519</v>
+        <v>489</v>
       </c>
       <c r="B61" s="1">
         <v>207089</v>
@@ -3850,13 +3426,10 @@
       <c r="G61" s="8">
         <v>1.2999999999999999E-3</v>
       </c>
-      <c r="H61" s="14" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>445</v>
+        <v>415</v>
       </c>
       <c r="B62" s="1">
         <v>7440417</v>
@@ -3876,13 +3449,10 @@
       <c r="G62" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="H62" s="8">
-        <v>200.8</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>494</v>
+        <v>464</v>
       </c>
       <c r="B63" s="1">
         <v>108601</v>
@@ -3902,13 +3472,10 @@
       <c r="G63" s="8">
         <v>1200</v>
       </c>
-      <c r="H63" s="14" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>520</v>
+        <v>490</v>
       </c>
       <c r="B64" s="1">
         <v>111911</v>
@@ -3928,13 +3495,10 @@
       <c r="G64" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H64" s="14" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>495</v>
+        <v>465</v>
       </c>
       <c r="B65" s="1">
         <v>111444</v>
@@ -3954,11 +3518,8 @@
       <c r="G65" s="8">
         <v>0.02</v>
       </c>
-      <c r="H65" s="14" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>381</v>
       </c>
@@ -3980,13 +3541,10 @@
       <c r="G66" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H66" s="8">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>446</v>
+        <v>416</v>
       </c>
       <c r="B67" s="15" t="s">
         <v>75</v>
@@ -4006,11 +3564,8 @@
       <c r="G67" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H67" s="14" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>61</v>
       </c>
@@ -4032,13 +3587,10 @@
       <c r="G68" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H68" s="8" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>496</v>
+        <v>466</v>
       </c>
       <c r="B69" s="1">
         <v>85687</v>
@@ -4058,13 +3610,10 @@
       <c r="G69" s="8">
         <v>190</v>
       </c>
-      <c r="H69" s="8" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>431</v>
+        <v>401</v>
       </c>
       <c r="B70" s="1">
         <v>7440439</v>
@@ -4084,13 +3633,10 @@
       <c r="G70" s="13">
         <v>0.24599634148460026</v>
       </c>
-      <c r="H70" s="8">
-        <v>200.8</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>447</v>
+        <v>417</v>
       </c>
       <c r="B71" s="1">
         <v>7440439</v>
@@ -4110,13 +3656,10 @@
       <c r="G71" s="13">
         <v>3.9221186109975661</v>
       </c>
-      <c r="H71" s="8">
-        <v>200.8</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>497</v>
+        <v>467</v>
       </c>
       <c r="B72" s="1">
         <v>56235</v>
@@ -4136,11 +3679,8 @@
       <c r="G72" s="8">
         <v>0.1</v>
       </c>
-      <c r="H72" s="8">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>284</v>
       </c>
@@ -4162,11 +3702,8 @@
       <c r="G73" s="8">
         <v>8.1000000000000004E-5</v>
       </c>
-      <c r="H73" s="8" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>342</v>
       </c>
@@ -4188,11 +3725,8 @@
       <c r="G74" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H74" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>98</v>
       </c>
@@ -4214,11 +3748,8 @@
       <c r="G75" s="8">
         <v>74</v>
       </c>
-      <c r="H75" s="8">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>100</v>
       </c>
@@ -4240,11 +3771,8 @@
       <c r="G76" s="8">
         <v>0.31</v>
       </c>
-      <c r="H76" s="8">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>102</v>
       </c>
@@ -4266,11 +3794,8 @@
       <c r="G77" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H77" s="8">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>106</v>
       </c>
@@ -4292,11 +3817,8 @@
       <c r="G78" s="8">
         <v>260</v>
       </c>
-      <c r="H78" s="8">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>375</v>
       </c>
@@ -4318,11 +3840,8 @@
       <c r="G79" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H79" s="8">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>286</v>
       </c>
@@ -4344,13 +3863,10 @@
       <c r="G80" s="8">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="H80" s="8" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>439</v>
+        <v>409</v>
       </c>
       <c r="B81" s="1">
         <v>16065831</v>
@@ -4370,13 +3886,10 @@
       <c r="G81" s="13">
         <v>74.114522080141811</v>
       </c>
-      <c r="H81" s="14" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>440</v>
+        <v>410</v>
       </c>
       <c r="B82" s="1">
         <v>18540299</v>
@@ -4396,13 +3909,10 @@
       <c r="G82" s="13">
         <v>10.581999999999999</v>
       </c>
-      <c r="H82" s="8">
-        <v>218.6</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>432</v>
+        <v>402</v>
       </c>
       <c r="B83" s="1">
         <v>7440473</v>
@@ -4422,13 +3932,10 @@
       <c r="G83" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="H83" s="8">
-        <v>200.8</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>448</v>
+        <v>418</v>
       </c>
       <c r="B84" s="1">
         <v>7440473</v>
@@ -4448,11 +3955,8 @@
       <c r="G84" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="H84" s="8">
-        <v>200.8</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>216</v>
       </c>
@@ -4474,13 +3978,10 @@
       <c r="G85" s="8">
         <v>1.2999999999999999E-3</v>
       </c>
-      <c r="H85" s="14" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>449</v>
+        <v>419</v>
       </c>
       <c r="B86" s="15" t="s">
         <v>77</v>
@@ -4500,13 +4001,10 @@
       <c r="G86" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H86" s="8">
-        <v>200.8</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>433</v>
+        <v>403</v>
       </c>
       <c r="B87" s="1">
         <v>7440508</v>
@@ -4526,13 +4024,10 @@
       <c r="G87" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="H87" s="8">
-        <v>200.8</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>450</v>
+        <v>420</v>
       </c>
       <c r="B88" s="1">
         <v>7440508</v>
@@ -4552,13 +4047,10 @@
       <c r="G88" s="13">
         <v>11.823841083208801</v>
       </c>
-      <c r="H88" s="8">
-        <v>200.8</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>464</v>
+        <v>434</v>
       </c>
       <c r="B89" s="2">
         <v>57125</v>
@@ -4578,13 +4070,10 @@
       <c r="G89" s="13">
         <v>130</v>
       </c>
-      <c r="H89" s="14" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>466</v>
+        <v>436</v>
       </c>
       <c r="B90" s="2" t="s">
         <v>60</v>
@@ -4604,11 +4093,8 @@
       <c r="G90" s="13">
         <v>5.2</v>
       </c>
-      <c r="H90" s="14" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>288</v>
       </c>
@@ -4630,13 +4116,10 @@
       <c r="G91" s="8">
         <v>0.1</v>
       </c>
-      <c r="H91" s="8" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>498</v>
+        <v>468</v>
       </c>
       <c r="B92" s="1">
         <v>117817</v>
@@ -4656,13 +4139,10 @@
       <c r="G92" s="8">
         <v>0.2</v>
       </c>
-      <c r="H92" s="14" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>521</v>
+        <v>491</v>
       </c>
       <c r="B93" s="1">
         <v>53703</v>
@@ -4682,13 +4162,10 @@
       <c r="G93" s="8">
         <v>1.2999999999999999E-3</v>
       </c>
-      <c r="H93" s="14" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>499</v>
+        <v>469</v>
       </c>
       <c r="B94" s="1">
         <v>84742</v>
@@ -4708,11 +4185,8 @@
       <c r="G94" s="8">
         <v>400</v>
       </c>
-      <c r="H94" s="8" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>108</v>
       </c>
@@ -4734,11 +4208,8 @@
       <c r="G95" s="8">
         <v>0.42</v>
       </c>
-      <c r="H95" s="8">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>382</v>
       </c>
@@ -4760,11 +4231,8 @@
       <c r="G96" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H96" s="8">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>296</v>
       </c>
@@ -4786,11 +4254,8 @@
       <c r="G97" s="8">
         <v>5.3000000000000001E-6</v>
       </c>
-      <c r="H97" s="8" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>226</v>
       </c>
@@ -4812,11 +4277,8 @@
       <c r="G98" s="8">
         <v>3800</v>
       </c>
-      <c r="H98" s="8" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>228</v>
       </c>
@@ -4838,11 +4300,8 @@
       <c r="G99" s="8">
         <v>84000</v>
       </c>
-      <c r="H99" s="8" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>220</v>
       </c>
@@ -4864,11 +4323,8 @@
       <c r="G100" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H100" s="8" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>304</v>
       </c>
@@ -4890,13 +4346,10 @@
       <c r="G101" s="8">
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="H101" s="8" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>500</v>
+        <v>470</v>
       </c>
       <c r="B102" s="1">
         <v>1031078</v>
@@ -4916,11 +4369,8 @@
       <c r="G102" s="8">
         <v>8.5</v>
       </c>
-      <c r="H102" s="8" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>306</v>
       </c>
@@ -4942,13 +4392,10 @@
       <c r="G103" s="8">
         <v>2.4E-2</v>
       </c>
-      <c r="H103" s="8" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>501</v>
+        <v>471</v>
       </c>
       <c r="B104" s="1">
         <v>7421934</v>
@@ -4968,11 +4415,8 @@
       <c r="G104" s="8">
         <v>0.03</v>
       </c>
-      <c r="H104" s="8" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>128</v>
       </c>
@@ -4994,11 +4438,8 @@
       <c r="G105" s="8">
         <v>160</v>
       </c>
-      <c r="H105" s="8">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>236</v>
       </c>
@@ -5020,11 +4461,8 @@
       <c r="G106" s="8">
         <v>14</v>
       </c>
-      <c r="H106" s="14" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>238</v>
       </c>
@@ -5046,11 +4484,8 @@
       <c r="G107" s="8">
         <v>390</v>
       </c>
-      <c r="H107" s="14" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>63</v>
       </c>
@@ -5072,11 +4507,8 @@
       <c r="G108" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H108" s="8" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>398</v>
       </c>
@@ -5098,11 +4530,8 @@
       <c r="G109" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H109" s="8">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>312</v>
       </c>
@@ -5124,13 +4553,10 @@
       <c r="G110" s="8">
         <v>7.9000000000000006E-6</v>
       </c>
-      <c r="H110" s="8" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>502</v>
+        <v>472</v>
       </c>
       <c r="B111" s="1">
         <v>1024573</v>
@@ -5150,11 +4576,8 @@
       <c r="G111" s="8">
         <v>3.8999999999999999E-6</v>
       </c>
-      <c r="H111" s="8" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>240</v>
       </c>
@@ -5176,11 +4599,8 @@
       <c r="G112" s="8">
         <v>2.9E-5</v>
       </c>
-      <c r="H112" s="14" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>242</v>
       </c>
@@ -5202,11 +4622,8 @@
       <c r="G113" s="8">
         <v>0.36</v>
       </c>
-      <c r="H113" s="14" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>244</v>
       </c>
@@ -5228,11 +4645,8 @@
       <c r="G114" s="8">
         <v>30</v>
       </c>
-      <c r="H114" s="14" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>246</v>
       </c>
@@ -5254,11 +4668,8 @@
       <c r="G115" s="8">
         <v>0.28999999999999998</v>
       </c>
-      <c r="H115" s="14" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>384</v>
       </c>
@@ -5280,13 +4691,10 @@
       <c r="G116" s="8">
         <v>2</v>
       </c>
-      <c r="H116" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
-        <v>528</v>
+        <v>498</v>
       </c>
       <c r="B117" s="1">
         <v>193395</v>
@@ -5306,11 +4714,8 @@
       <c r="G117" s="8">
         <v>1.2999999999999999E-3</v>
       </c>
-      <c r="H117" s="8" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>376</v>
       </c>
@@ -5332,13 +4737,10 @@
       <c r="G118" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H118" s="14" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
-        <v>451</v>
+        <v>421</v>
       </c>
       <c r="B119" s="1">
         <v>7439896</v>
@@ -5358,11 +4760,8 @@
       <c r="G119" s="13">
         <v>1000</v>
       </c>
-      <c r="H119" s="14" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>250</v>
       </c>
@@ -5384,13 +4783,10 @@
       <c r="G120" s="8">
         <v>27</v>
       </c>
-      <c r="H120" s="8" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
-        <v>434</v>
+        <v>404</v>
       </c>
       <c r="B121" s="1">
         <v>7439921</v>
@@ -5410,13 +4806,10 @@
       <c r="G121" s="13">
         <v>2.5166437242964461</v>
       </c>
-      <c r="H121" s="8">
-        <v>200.8</v>
-      </c>
-    </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
-        <v>452</v>
+        <v>422</v>
       </c>
       <c r="B122" s="1">
         <v>7439921</v>
@@ -5436,13 +4829,10 @@
       <c r="G122" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="H122" s="8">
-        <v>200.8</v>
-      </c>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
-        <v>529</v>
+        <v>499</v>
       </c>
       <c r="B123" s="1">
         <v>58899</v>
@@ -5462,13 +4852,10 @@
       <c r="G123" s="8">
         <v>0.08</v>
       </c>
-      <c r="H123" s="8" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
-        <v>453</v>
+        <v>423</v>
       </c>
       <c r="B124" s="15" t="s">
         <v>79</v>
@@ -5488,11 +4875,8 @@
       <c r="G124" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H124" s="14" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>316</v>
       </c>
@@ -5514,13 +4898,10 @@
       <c r="G125" s="8">
         <v>0.1</v>
       </c>
-      <c r="H125" s="14" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>454</v>
+        <v>424</v>
       </c>
       <c r="B126" s="15" t="s">
         <v>83</v>
@@ -5540,13 +4921,10 @@
       <c r="G126" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H126" s="14" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
-        <v>530</v>
+        <v>500</v>
       </c>
       <c r="B127" s="1">
         <v>541731</v>
@@ -5566,13 +4944,10 @@
       <c r="G127" s="8">
         <v>80</v>
       </c>
-      <c r="H127" s="8">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
-        <v>463</v>
+        <v>433</v>
       </c>
       <c r="B128" s="1">
         <v>7439976</v>
@@ -5592,11 +4967,8 @@
       <c r="G128" s="18">
         <v>1.2E-2</v>
       </c>
-      <c r="H128" s="8" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>318</v>
       </c>
@@ -5618,13 +4990,10 @@
       <c r="G129" s="8">
         <v>0.03</v>
       </c>
-      <c r="H129" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="B130" s="1">
         <v>74839</v>
@@ -5644,13 +5013,10 @@
       <c r="G130" s="8">
         <v>37</v>
       </c>
-      <c r="H130" s="8">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
-        <v>504</v>
+        <v>474</v>
       </c>
       <c r="B131" s="1">
         <v>75092</v>
@@ -5670,11 +5036,8 @@
       <c r="G131" s="8">
         <v>4.3</v>
       </c>
-      <c r="H131" s="8">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>385</v>
       </c>
@@ -5696,11 +5059,8 @@
       <c r="G132" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="H132" s="8">
-        <v>1630</v>
-      </c>
-    </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>320</v>
       </c>
@@ -5722,13 +5082,10 @@
       <c r="G133" s="8">
         <v>1E-3</v>
       </c>
-      <c r="H133" s="8">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
-        <v>455</v>
+        <v>425</v>
       </c>
       <c r="B134" s="15" t="s">
         <v>81</v>
@@ -5748,13 +5105,10 @@
       <c r="G134" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H134" s="14" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>531</v>
+        <v>501</v>
       </c>
       <c r="B135" s="1">
         <v>91203</v>
@@ -5774,13 +5128,10 @@
       <c r="G135" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H135" s="8" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>435</v>
+        <v>405</v>
       </c>
       <c r="B136" s="1">
         <v>7440020</v>
@@ -5800,13 +5151,10 @@
       <c r="G136" s="13">
         <v>52.006539397853551</v>
       </c>
-      <c r="H136" s="8">
-        <v>200.8</v>
-      </c>
-    </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>456</v>
+        <v>426</v>
       </c>
       <c r="B137" s="1">
         <v>7440020</v>
@@ -5826,13 +5174,10 @@
       <c r="G137" s="13">
         <v>140</v>
       </c>
-      <c r="H137" s="8">
-        <v>200.8</v>
-      </c>
-    </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>532</v>
+        <v>502</v>
       </c>
       <c r="B138" s="1">
         <v>14797558</v>
@@ -5852,11 +5197,8 @@
       <c r="G138" s="8">
         <v>10000</v>
       </c>
-      <c r="H138" s="14" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
         <v>377</v>
       </c>
@@ -5878,11 +5220,8 @@
       <c r="G139" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H139" s="14" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
         <v>254</v>
       </c>
@@ -5904,11 +5243,8 @@
       <c r="G140" s="8">
         <v>14</v>
       </c>
-      <c r="H140" s="8" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>354</v>
       </c>
@@ -5930,13 +5266,10 @@
       <c r="G141" s="8">
         <v>7.9000000000000001E-4</v>
       </c>
-      <c r="H141" s="8">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>533</v>
+        <v>503</v>
       </c>
       <c r="B142" s="1">
         <v>62759</v>
@@ -5956,11 +5289,8 @@
       <c r="G142" s="8">
         <v>6.8000000000000005E-4</v>
       </c>
-      <c r="H142" s="14" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
         <v>387</v>
       </c>
@@ -5982,13 +5312,10 @@
       <c r="G143" s="8">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="H143" s="8">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
-        <v>534</v>
+        <v>504</v>
       </c>
       <c r="B144" s="1">
         <v>621647</v>
@@ -6008,13 +5335,10 @@
       <c r="G144" s="8">
         <v>4.5999999999999999E-3</v>
       </c>
-      <c r="H144" s="14" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
-        <v>535</v>
+        <v>505</v>
       </c>
       <c r="B145" s="1">
         <v>86306</v>
@@ -6034,11 +5358,8 @@
       <c r="G145" s="8">
         <v>0.55000000000000004</v>
       </c>
-      <c r="H145" s="14" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
         <v>356</v>
       </c>
@@ -6060,13 +5381,10 @@
       <c r="G146" s="8">
         <v>1.6E-2</v>
       </c>
-      <c r="H146" s="8">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
-        <v>525</v>
+        <v>495</v>
       </c>
       <c r="B147" s="1">
         <v>95578</v>
@@ -6086,13 +5404,10 @@
       <c r="G147" s="8">
         <v>14</v>
       </c>
-      <c r="H147" s="8" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
-        <v>524</v>
+        <v>494</v>
       </c>
       <c r="B148" s="1">
         <v>95501</v>
@@ -6112,13 +5427,10 @@
       <c r="G148" s="8">
         <v>110</v>
       </c>
-      <c r="H148" s="8">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
-        <v>523</v>
+        <v>493</v>
       </c>
       <c r="B149" s="1">
         <v>88755</v>
@@ -6138,13 +5450,10 @@
       <c r="G149" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H149" s="8" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
-        <v>522</v>
+        <v>492</v>
       </c>
       <c r="B150" s="1">
         <v>72548</v>
@@ -6164,13 +5473,10 @@
       <c r="G150" s="8">
         <v>3.1000000000000001E-5</v>
       </c>
-      <c r="H150" s="8" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
-        <v>526</v>
+        <v>496</v>
       </c>
       <c r="B151" s="1">
         <v>72559</v>
@@ -6190,13 +5496,10 @@
       <c r="G151" s="8">
         <v>2.1999999999999999E-5</v>
       </c>
-      <c r="H151" s="8" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
-        <v>527</v>
+        <v>497</v>
       </c>
       <c r="B152" s="1">
         <v>50293</v>
@@ -6216,11 +5519,8 @@
       <c r="G152" s="8">
         <v>2.1999999999999999E-5</v>
       </c>
-      <c r="H152" s="8" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>322</v>
       </c>
@@ -6242,13 +5542,10 @@
       <c r="G153" s="8">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="H153" s="8">
-        <v>614</v>
-      </c>
-    </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
-        <v>505</v>
+        <v>475</v>
       </c>
       <c r="B154" s="1">
         <v>101553</v>
@@ -6268,13 +5565,10 @@
       <c r="G154" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H154" s="8" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
-        <v>536</v>
+        <v>506</v>
       </c>
       <c r="B155" s="1">
         <v>59507</v>
@@ -6294,13 +5588,10 @@
       <c r="G155" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H155" s="8" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
-        <v>506</v>
+        <v>476</v>
       </c>
       <c r="B156" s="1">
         <v>7005723</v>
@@ -6320,13 +5611,10 @@
       <c r="G156" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H156" s="8" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
-        <v>537</v>
+        <v>507</v>
       </c>
       <c r="B157" s="1">
         <v>106467</v>
@@ -6346,11 +5634,8 @@
       <c r="G157" s="8">
         <v>16</v>
       </c>
-      <c r="H157" s="8">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
         <v>262</v>
       </c>
@@ -6372,11 +5657,8 @@
       <c r="G158" s="8">
         <v>0.15</v>
       </c>
-      <c r="H158" s="8" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
         <v>172</v>
       </c>
@@ -6398,11 +5680,8 @@
       <c r="G159" s="8">
         <v>0.15</v>
       </c>
-      <c r="H159" s="14" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
         <v>264</v>
       </c>
@@ -6424,11 +5703,8 @@
       <c r="G160" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H160" s="14" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
         <v>174</v>
       </c>
@@ -6450,11 +5726,8 @@
       <c r="G161" s="8">
         <v>9400</v>
       </c>
-      <c r="H161" s="8" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
         <v>396</v>
       </c>
@@ -6476,11 +5749,8 @@
       <c r="G162" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="H162" s="8">
-        <v>420.1</v>
-      </c>
-    </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
         <v>388</v>
       </c>
@@ -6502,13 +5772,10 @@
       <c r="G163" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H163" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
-        <v>538</v>
+        <v>508</v>
       </c>
       <c r="B164" s="1">
         <v>100027</v>
@@ -6528,11 +5795,8 @@
       <c r="G164" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H164" s="8" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
         <v>266</v>
       </c>
@@ -6554,13 +5818,10 @@
       <c r="G165" s="8">
         <v>290</v>
       </c>
-      <c r="H165" s="14" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
-        <v>436</v>
+        <v>406</v>
       </c>
       <c r="B166" s="1">
         <v>7782492</v>
@@ -6580,13 +5841,10 @@
       <c r="G166" s="13">
         <v>4.2412000000000001</v>
       </c>
-      <c r="H166" s="8">
-        <v>200.8</v>
-      </c>
-    </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
-        <v>457</v>
+        <v>427</v>
       </c>
       <c r="B167" s="1">
         <v>7782492</v>
@@ -6606,13 +5864,10 @@
       <c r="G167" s="13">
         <v>120</v>
       </c>
-      <c r="H167" s="8">
-        <v>200.8</v>
-      </c>
-    </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
-        <v>437</v>
+        <v>407</v>
       </c>
       <c r="B168" s="1">
         <v>7440224</v>
@@ -6632,13 +5887,10 @@
       <c r="G168" s="13">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="H168" s="8">
-        <v>200.8</v>
-      </c>
-    </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
-        <v>458</v>
+        <v>428</v>
       </c>
       <c r="B169" s="1">
         <v>7440224</v>
@@ -6658,11 +5910,8 @@
       <c r="G169" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="H169" s="8">
-        <v>200.8</v>
-      </c>
-    </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
         <v>378</v>
       </c>
@@ -6684,11 +5933,8 @@
       <c r="G170" s="8">
         <v>10</v>
       </c>
-      <c r="H170" s="14" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
         <v>65</v>
       </c>
@@ -6710,11 +5956,8 @@
       <c r="G171" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H171" s="8" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
         <v>389</v>
       </c>
@@ -6736,11 +5979,8 @@
       <c r="G172" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H172" s="8" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
         <v>391</v>
       </c>
@@ -6762,11 +6002,8 @@
       <c r="G173" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H173" s="14" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
         <v>392</v>
       </c>
@@ -6788,11 +6025,8 @@
       <c r="G174" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H174" s="14" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
         <v>393</v>
       </c>
@@ -6814,11 +6048,8 @@
       <c r="G175" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H175" s="14" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
         <v>394</v>
       </c>
@@ -6840,11 +6071,8 @@
       <c r="G176" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H176" s="14" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
         <v>395</v>
       </c>
@@ -6866,11 +6094,8 @@
       <c r="G177" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H177" s="14" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
         <v>138</v>
       </c>
@@ -6892,13 +6117,10 @@
       <c r="G178" s="8">
         <v>0.24</v>
       </c>
-      <c r="H178" s="8">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
-        <v>459</v>
+        <v>429</v>
       </c>
       <c r="B179" s="1">
         <v>7440280</v>
@@ -6918,13 +6140,10 @@
       <c r="G179" s="12">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="H179" s="8">
-        <v>200.8</v>
-      </c>
-    </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
-        <v>460</v>
+        <v>430</v>
       </c>
       <c r="B180" s="15" t="s">
         <v>85</v>
@@ -6944,13 +6163,10 @@
       <c r="G180" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H180" s="8">
-        <v>200.8</v>
-      </c>
-    </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
-        <v>461</v>
+        <v>431</v>
       </c>
       <c r="B181" s="15" t="s">
         <v>87</v>
@@ -6970,11 +6186,8 @@
       <c r="G181" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H181" s="8">
-        <v>200.8</v>
-      </c>
-    </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
         <v>140</v>
       </c>
@@ -6996,11 +6209,8 @@
       <c r="G182" s="8">
         <v>720</v>
       </c>
-      <c r="H182" s="8">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
         <v>326</v>
       </c>
@@ -7022,11 +6232,8 @@
       <c r="G183" s="8">
         <v>6.3999999999999997E-6</v>
       </c>
-      <c r="H183" s="8" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
         <v>324</v>
       </c>
@@ -7048,13 +6255,10 @@
       <c r="G184" s="8">
         <v>2.8E-5</v>
       </c>
-      <c r="H184" s="14" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
-        <v>476</v>
+        <v>446</v>
       </c>
       <c r="B185" s="1">
         <v>156605</v>
@@ -7074,13 +6278,10 @@
       <c r="G185" s="8">
         <v>120</v>
       </c>
-      <c r="H185" s="8">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
-        <v>475</v>
+        <v>445</v>
       </c>
       <c r="B186" s="1">
         <v>75252</v>
@@ -7100,11 +6301,8 @@
       <c r="G186" s="8">
         <v>3.3</v>
       </c>
-      <c r="H186" s="8">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
         <v>397</v>
       </c>
@@ -7126,13 +6324,10 @@
       <c r="G187" s="8">
         <v>6.3E-2</v>
       </c>
-      <c r="H187" s="14" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
-        <v>474</v>
+        <v>444</v>
       </c>
       <c r="B188" s="1">
         <v>79016</v>
@@ -7152,13 +6347,10 @@
       <c r="G188" s="8">
         <v>1.4</v>
       </c>
-      <c r="H188" s="8">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
-        <v>473</v>
+        <v>443</v>
       </c>
       <c r="B189" s="1">
         <v>75014</v>
@@ -7178,13 +6370,10 @@
       <c r="G189" s="8">
         <v>2.3E-2</v>
       </c>
-      <c r="H189" s="8">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
-        <v>438</v>
+        <v>408</v>
       </c>
       <c r="B190" s="1">
         <v>7440666</v>
@@ -7204,13 +6393,10 @@
       <c r="G190" s="13">
         <v>117.18045413475284</v>
       </c>
-      <c r="H190" s="8">
-        <v>200.8</v>
-      </c>
-    </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
-        <v>462</v>
+        <v>432</v>
       </c>
       <c r="B191" s="1">
         <v>7440666</v>
@@ -7230,48 +6416,9 @@
       <c r="G191" s="13">
         <v>2100</v>
       </c>
-      <c r="H191" s="8">
-        <v>200.8</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H191">
-    <sortState ref="A2:H191">
-      <sortCondition ref="A1:A191"/>
-    </sortState>
-  </autoFilter>
-  <conditionalFormatting sqref="H2:H34 H36:H38 H41:H191">
-    <cfRule type="containsText" dxfId="7" priority="15" operator="containsText" text="&gt;WQC">
-      <formula>NOT(ISERROR(SEARCH("&gt;WQC",H2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="16" operator="containsText" text="ok">
-      <formula>NOT(ISERROR(SEARCH("ok",H2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H39">
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="&gt;WQC">
-      <formula>NOT(ISERROR(SEARCH("&gt;WQC",H39)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="ok">
-      <formula>NOT(ISERROR(SEARCH("ok",H39)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H40">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="&gt;WQC">
-      <formula>NOT(ISERROR(SEARCH("&gt;WQC",H40)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="ok">
-      <formula>NOT(ISERROR(SEARCH("ok",H40)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H35">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="&gt;WQC">
-      <formula>NOT(ISERROR(SEARCH("&gt;WQC",H35)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="ok">
-      <formula>NOT(ISERROR(SEARCH("ok",H35)))</formula>
-    </cfRule>
-  </conditionalFormatting>
+  <autoFilter ref="A1:G191"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Updates to QLs based on new memo 11/3/2020
</commit_message>
<xml_diff>
--- a/2_21_19_QLs.xlsx
+++ b/2_21_19_QLs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\deqlab1\WQDataSteward\R_Scripts\EDD_Data_QC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\EDD_Data_QC\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="526">
   <si>
     <t>Nitrates-Nitrite (as N)</t>
   </si>
@@ -1581,6 +1581,30 @@
   </si>
   <si>
     <t>Aluminum, Dissolved</t>
+  </si>
+  <si>
+    <t>Total Suspended Solids</t>
+  </si>
+  <si>
+    <t>Total Residual Chlorine</t>
+  </si>
+  <si>
+    <t>Oil and Grease</t>
+  </si>
+  <si>
+    <t>Total BTEX</t>
+  </si>
+  <si>
+    <t>Ammonia, Total (as N)</t>
+  </si>
+  <si>
+    <t>Chlorine, Total Residual</t>
+  </si>
+  <si>
+    <t>Ammonia</t>
+  </si>
+  <si>
+    <t>BTEX, Total</t>
   </si>
 </sst>
 </file>
@@ -1592,7 +1616,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1614,6 +1638,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1640,7 +1671,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1709,6 +1740,15 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1991,11 +2031,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V200"/>
+  <dimension ref="A1:V205"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A117" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B192" sqref="B192:G200"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C206" sqref="C206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2047,7 +2087,7 @@
         <v>299</v>
       </c>
       <c r="E2" s="8">
-        <v>0.01</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>364</v>
@@ -2093,7 +2133,7 @@
         <v>301</v>
       </c>
       <c r="E4" s="8">
-        <v>0.01</v>
+        <v>1.2E-2</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>364</v>
@@ -2185,7 +2225,7 @@
         <v>145</v>
       </c>
       <c r="E8" s="8">
-        <v>0.5</v>
+        <v>11.4</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>364</v>
@@ -2208,7 +2248,7 @@
         <v>117</v>
       </c>
       <c r="E9" s="8">
-        <v>0.5</v>
+        <v>14.1</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>364</v>
@@ -2231,7 +2271,7 @@
         <v>123</v>
       </c>
       <c r="E10" s="8">
-        <v>0.5</v>
+        <v>8.4</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>364</v>
@@ -2300,7 +2340,7 @@
         <v>269</v>
       </c>
       <c r="E13" s="12">
-        <v>1</v>
+        <v>5.7</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>364</v>
@@ -2415,7 +2455,7 @@
         <v>351</v>
       </c>
       <c r="E18" s="8">
-        <v>1.0000000000000001E-5</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>364</v>
@@ -2438,7 +2478,7 @@
         <v>177</v>
       </c>
       <c r="E19" s="13">
-        <v>2</v>
+        <v>165</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>364</v>
@@ -2507,7 +2547,7 @@
         <v>161</v>
       </c>
       <c r="E22" s="13">
-        <v>1</v>
+        <v>8.1</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>364</v>
@@ -2530,7 +2570,7 @@
         <v>163</v>
       </c>
       <c r="E23" s="13">
-        <v>5</v>
+        <v>8.1</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>364</v>
@@ -2553,7 +2593,7 @@
         <v>167</v>
       </c>
       <c r="E24" s="13">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>364</v>
@@ -2599,7 +2639,7 @@
         <v>233</v>
       </c>
       <c r="E26" s="12">
-        <v>1</v>
+        <v>5.7</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>364</v>
@@ -2645,7 +2685,7 @@
         <v>213</v>
       </c>
       <c r="E28" s="13">
-        <v>1</v>
+        <v>5.7</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>364</v>
@@ -2668,7 +2708,7 @@
         <v>225</v>
       </c>
       <c r="E29" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>364</v>
@@ -2691,7 +2731,7 @@
         <v>165</v>
       </c>
       <c r="E30" s="13">
-        <v>2</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>364</v>
@@ -2714,7 +2754,7 @@
         <v>181</v>
       </c>
       <c r="E31" s="13">
-        <v>1</v>
+        <v>5.7</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>364</v>
@@ -2737,7 +2777,7 @@
         <v>183</v>
       </c>
       <c r="E32" s="13">
-        <v>1</v>
+        <v>10.5</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>364</v>
@@ -2898,7 +2938,7 @@
         <v>185</v>
       </c>
       <c r="E39" s="13">
-        <v>1</v>
+        <v>5.7</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>364</v>
@@ -3174,7 +3214,7 @@
         <v>311</v>
       </c>
       <c r="E51" s="8">
-        <v>1</v>
+        <v>1.75</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>364</v>
@@ -3197,7 +3237,7 @@
         <v>187</v>
       </c>
       <c r="E52" s="13">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>364</v>
@@ -3335,7 +3375,7 @@
         <v>189</v>
       </c>
       <c r="E58" s="8">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="F58" s="2" t="s">
         <v>364</v>
@@ -3404,7 +3444,7 @@
         <v>197</v>
       </c>
       <c r="E61" s="12">
-        <v>1</v>
+        <v>12.3</v>
       </c>
       <c r="F61" s="2" t="s">
         <v>364</v>
@@ -3427,7 +3467,7 @@
         <v>199</v>
       </c>
       <c r="E62" s="12">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F62" s="2" t="s">
         <v>364</v>
@@ -3450,7 +3490,7 @@
         <v>11</v>
       </c>
       <c r="E63" s="12">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="F63" s="2" t="s">
         <v>364</v>
@@ -3473,7 +3513,7 @@
         <v>205</v>
       </c>
       <c r="E64" s="13">
-        <v>2</v>
+        <v>17.100000000000001</v>
       </c>
       <c r="F64" s="2" t="s">
         <v>364</v>
@@ -3496,7 +3536,7 @@
         <v>201</v>
       </c>
       <c r="E65" s="13">
-        <v>2</v>
+        <v>15.9</v>
       </c>
       <c r="F65" s="2" t="s">
         <v>364</v>
@@ -3611,7 +3651,7 @@
         <v>211</v>
       </c>
       <c r="E70" s="13">
-        <v>1</v>
+        <v>7.5</v>
       </c>
       <c r="F70" s="2" t="s">
         <v>364</v>
@@ -3634,7 +3674,7 @@
         <v>13</v>
       </c>
       <c r="E71" s="12">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="F71" s="2" t="s">
         <v>364</v>
@@ -3657,7 +3697,7 @@
         <v>13</v>
       </c>
       <c r="E72" s="12">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="F72" s="2" t="s">
         <v>364</v>
@@ -3772,7 +3812,7 @@
         <v>99</v>
       </c>
       <c r="E77" s="8">
-        <v>0.5</v>
+        <v>18</v>
       </c>
       <c r="F77" s="2" t="s">
         <v>364</v>
@@ -3818,7 +3858,7 @@
         <v>103</v>
       </c>
       <c r="E79" s="8">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="F79" s="2" t="s">
         <v>364</v>
@@ -3841,7 +3881,7 @@
         <v>107</v>
       </c>
       <c r="E80" s="8">
-        <v>0.5</v>
+        <v>4.8</v>
       </c>
       <c r="F80" s="2" t="s">
         <v>364</v>
@@ -3887,7 +3927,7 @@
         <v>287</v>
       </c>
       <c r="E82" s="8">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="F82" s="2" t="s">
         <v>364</v>
@@ -3979,7 +4019,7 @@
         <v>16</v>
       </c>
       <c r="E86" s="12">
-        <v>0.4</v>
+        <v>2</v>
       </c>
       <c r="F86" s="2" t="s">
         <v>364</v>
@@ -4140,7 +4180,7 @@
         <v>58</v>
       </c>
       <c r="E93" s="13">
-        <v>5</v>
+        <v>7.2</v>
       </c>
       <c r="F93" s="2" t="s">
         <v>364</v>
@@ -4162,8 +4202,8 @@
       <c r="D94" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="E94" s="13">
-        <v>2</v>
+      <c r="E94" s="12">
+        <v>2.4500000000000002</v>
       </c>
       <c r="F94" s="2" t="s">
         <v>364</v>
@@ -4185,8 +4225,8 @@
       <c r="D95" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="E95" s="13">
-        <v>1</v>
+      <c r="E95" s="12">
+        <v>7.25</v>
       </c>
       <c r="F95" s="2" t="s">
         <v>364</v>
@@ -4232,7 +4272,7 @@
         <v>219</v>
       </c>
       <c r="E97" s="13">
-        <v>1</v>
+        <v>7.5</v>
       </c>
       <c r="F97" s="2" t="s">
         <v>364</v>
@@ -4324,7 +4364,7 @@
         <v>227</v>
       </c>
       <c r="E101" s="13">
-        <v>1</v>
+        <v>5.7</v>
       </c>
       <c r="F101" s="2" t="s">
         <v>364</v>
@@ -4347,7 +4387,7 @@
         <v>229</v>
       </c>
       <c r="E102" s="13">
-        <v>1</v>
+        <v>4.8</v>
       </c>
       <c r="F102" s="2" t="s">
         <v>364</v>
@@ -4370,7 +4410,7 @@
         <v>221</v>
       </c>
       <c r="E103" s="13">
-        <v>1</v>
+        <v>7.5</v>
       </c>
       <c r="F103" s="2" t="s">
         <v>364</v>
@@ -4416,7 +4456,7 @@
         <v>303</v>
       </c>
       <c r="E105" s="8">
-        <v>0.01</v>
+        <v>0.19800000000000001</v>
       </c>
       <c r="F105" s="2" t="s">
         <v>364</v>
@@ -4439,7 +4479,7 @@
         <v>307</v>
       </c>
       <c r="E106" s="8">
-        <v>0.01</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="F106" s="2" t="s">
         <v>364</v>
@@ -4462,7 +4502,7 @@
         <v>309</v>
       </c>
       <c r="E107" s="8">
-        <v>0.01</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="F107" s="2" t="s">
         <v>364</v>
@@ -4485,7 +4525,7 @@
         <v>129</v>
       </c>
       <c r="E108" s="8">
-        <v>0.5</v>
+        <v>21.6</v>
       </c>
       <c r="F108" s="2" t="s">
         <v>364</v>
@@ -4508,7 +4548,7 @@
         <v>237</v>
       </c>
       <c r="E109" s="13">
-        <v>2</v>
+        <v>6.6</v>
       </c>
       <c r="F109" s="2" t="s">
         <v>364</v>
@@ -4531,7 +4571,7 @@
         <v>239</v>
       </c>
       <c r="E110" s="13">
-        <v>1</v>
+        <v>5.7</v>
       </c>
       <c r="F110" s="2" t="s">
         <v>364</v>
@@ -4692,7 +4732,7 @@
         <v>245</v>
       </c>
       <c r="E117" s="13">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F117" s="2" t="s">
         <v>364</v>
@@ -4830,7 +4870,7 @@
         <v>251</v>
       </c>
       <c r="E123" s="13">
-        <v>5</v>
+        <v>6.6</v>
       </c>
       <c r="F123" s="2" t="s">
         <v>364</v>
@@ -4899,7 +4939,7 @@
         <v>283</v>
       </c>
       <c r="E126" s="8">
-        <v>0.01</v>
+        <v>1.2E-2</v>
       </c>
       <c r="F126" s="2" t="s">
         <v>364</v>
@@ -4945,7 +4985,7 @@
         <v>317</v>
       </c>
       <c r="E128" s="8">
-        <v>0.2</v>
+        <v>1.9</v>
       </c>
       <c r="F128" s="2" t="s">
         <v>364</v>
@@ -4991,7 +5031,7 @@
         <v>113</v>
       </c>
       <c r="E130" s="8">
-        <v>0.5</v>
+        <v>7.6</v>
       </c>
       <c r="F130" s="2" t="s">
         <v>364</v>
@@ -5083,7 +5123,7 @@
         <v>135</v>
       </c>
       <c r="E134" s="13">
-        <v>2</v>
+        <v>8.4</v>
       </c>
       <c r="F134" s="2" t="s">
         <v>364</v>
@@ -5129,7 +5169,7 @@
         <v>321</v>
       </c>
       <c r="E136" s="8">
-        <v>0.01</v>
+        <v>0.96</v>
       </c>
       <c r="F136" s="2" t="s">
         <v>364</v>
@@ -5175,7 +5215,7 @@
         <v>253</v>
       </c>
       <c r="E138" s="13">
-        <v>1</v>
+        <v>4.8</v>
       </c>
       <c r="F138" s="2" t="s">
         <v>364</v>
@@ -5290,7 +5330,7 @@
         <v>255</v>
       </c>
       <c r="E143" s="13">
-        <v>1</v>
+        <v>5.7</v>
       </c>
       <c r="F143" s="2" t="s">
         <v>364</v>
@@ -5336,7 +5376,7 @@
         <v>257</v>
       </c>
       <c r="E145" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F145" s="2" t="s">
         <v>364</v>
@@ -5451,7 +5491,7 @@
         <v>159</v>
       </c>
       <c r="E150" s="13">
-        <v>1</v>
+        <v>9.9</v>
       </c>
       <c r="F150" s="2" t="s">
         <v>364</v>
@@ -5474,7 +5514,7 @@
         <v>111</v>
       </c>
       <c r="E151" s="8">
-        <v>0.5</v>
+        <v>7.6</v>
       </c>
       <c r="F151" s="2" t="s">
         <v>364</v>
@@ -5497,7 +5537,7 @@
         <v>169</v>
       </c>
       <c r="E152" s="13">
-        <v>2</v>
+        <v>10.8</v>
       </c>
       <c r="F152" s="2" t="s">
         <v>364</v>
@@ -5612,7 +5652,7 @@
         <v>323</v>
       </c>
       <c r="E157" s="8">
-        <v>10</v>
+        <v>0.95</v>
       </c>
       <c r="F157" s="2" t="s">
         <v>364</v>
@@ -5635,7 +5675,7 @@
         <v>209</v>
       </c>
       <c r="E158" s="13">
-        <v>1</v>
+        <v>5.7</v>
       </c>
       <c r="F158" s="2" t="s">
         <v>364</v>
@@ -5658,7 +5698,7 @@
         <v>157</v>
       </c>
       <c r="E159" s="13">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="F159" s="2" t="s">
         <v>364</v>
@@ -5681,7 +5721,7 @@
         <v>215</v>
       </c>
       <c r="E160" s="13">
-        <v>1</v>
+        <v>12.6</v>
       </c>
       <c r="F160" s="2" t="s">
         <v>364</v>
@@ -5704,7 +5744,7 @@
         <v>115</v>
       </c>
       <c r="E161" s="8">
-        <v>0.5</v>
+        <v>8</v>
       </c>
       <c r="F161" s="2" t="s">
         <v>364</v>
@@ -5796,7 +5836,7 @@
         <v>265</v>
       </c>
       <c r="E165" s="12">
-        <v>1</v>
+        <v>16.2</v>
       </c>
       <c r="F165" s="2" t="s">
         <v>364</v>
@@ -5819,7 +5859,7 @@
         <v>175</v>
       </c>
       <c r="E166" s="13">
-        <v>1</v>
+        <v>4.5</v>
       </c>
       <c r="F166" s="2" t="s">
         <v>364</v>
@@ -5842,7 +5882,7 @@
         <v>60</v>
       </c>
       <c r="E167" s="8">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="F167" s="2" t="s">
         <v>364</v>
@@ -5888,7 +5928,7 @@
         <v>171</v>
       </c>
       <c r="E169" s="13">
-        <v>5</v>
+        <v>7.2</v>
       </c>
       <c r="F169" s="2" t="s">
         <v>364</v>
@@ -5934,7 +5974,7 @@
         <v>267</v>
       </c>
       <c r="E171" s="13">
-        <v>1</v>
+        <v>5.7</v>
       </c>
       <c r="F171" s="2" t="s">
         <v>364</v>
@@ -6371,7 +6411,7 @@
         <v>141</v>
       </c>
       <c r="E190" s="8">
-        <v>0.5</v>
+        <v>18</v>
       </c>
       <c r="F190" s="2" t="s">
         <v>364</v>
@@ -6463,7 +6503,7 @@
         <v>121</v>
       </c>
       <c r="E194" s="8">
-        <v>0.5</v>
+        <v>4.8</v>
       </c>
       <c r="F194" s="2" t="s">
         <v>364</v>
@@ -6608,6 +6648,76 @@
       </c>
       <c r="G200" s="13">
         <v>2100</v>
+      </c>
+    </row>
+    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A201" s="2" t="s">
+        <v>518</v>
+      </c>
+      <c r="C201" s="19" t="s">
+        <v>518</v>
+      </c>
+      <c r="E201" s="20">
+        <v>5</v>
+      </c>
+      <c r="F201" s="2" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A202" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="C202" s="19" t="s">
+        <v>519</v>
+      </c>
+      <c r="E202" s="20">
+        <v>50</v>
+      </c>
+      <c r="F202" s="2" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A203" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="C203" s="19" t="s">
+        <v>520</v>
+      </c>
+      <c r="E203" s="21">
+        <v>5000</v>
+      </c>
+      <c r="F203" s="2" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A204" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="C204" s="19" t="s">
+        <v>521</v>
+      </c>
+      <c r="E204" s="20">
+        <v>2</v>
+      </c>
+      <c r="F204" s="2" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A205" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="C205" s="19" t="s">
+        <v>522</v>
+      </c>
+      <c r="E205" s="20">
+        <v>20</v>
+      </c>
+      <c r="F205" s="2" t="s">
+        <v>364</v>
       </c>
     </row>
   </sheetData>

</xml_diff>